<commit_message>
Added weather to models, code, testcases
</commit_message>
<xml_diff>
--- a/Code/Overlap/Input Files/Experiment setups.xlsx
+++ b/Code/Overlap/Input Files/Experiment setups.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB540693-B763-494D-B7A1-27457A8C20B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F544DD-287A-4856-81A4-D8DB5B66D595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attempt 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attempt 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Variable</t>
   </si>
@@ -480,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08CA528-35B9-41F9-81F2-1C5E6595BF4E}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,4 +826,354 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AD7D99-8775-4118-A1C8-7FD1490F7E75}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>PRODUCT(J2:J5)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:F17" si="0">B$13/100*$H14</f>
+        <v>3.6</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="H14">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>6.72</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>33.6</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>67.2</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="H15">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="H16">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="H17">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new setup ideas
</commit_message>
<xml_diff>
--- a/Code/Overlap/Input Files/Experiment setups.xlsx
+++ b/Code/Overlap/Input Files/Experiment setups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F544DD-287A-4856-81A4-D8DB5B66D595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1812D8E-58E3-4977-B5E5-A22E9F6FAEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Variable</t>
   </si>
@@ -104,6 +104,126 @@
   </si>
   <si>
     <t>Constant, wave, binary</t>
+  </si>
+  <si>
+    <t>No FSV</t>
+  </si>
+  <si>
+    <t>Only CTV</t>
+  </si>
+  <si>
+    <t>CTV + Tech</t>
+  </si>
+  <si>
+    <t>No Tech</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>(None)</t>
+  </si>
+  <si>
+    <t>All (None)</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>Seasonal</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>1 summer</t>
+  </si>
+  <si>
+    <t>2 summers (3m wint)</t>
+  </si>
+  <si>
+    <t>2 summers (6m wint)</t>
+  </si>
+  <si>
+    <t>3 summers (3m wint)</t>
+  </si>
+  <si>
+    <t>3 summers (6m wint)</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>2 years</t>
+  </si>
+  <si>
+    <t>6+6+6</t>
+  </si>
+  <si>
+    <t>9+3+9</t>
+  </si>
+  <si>
+    <t>9+3+9+3+9</t>
+  </si>
+  <si>
+    <t>6+6+6+6+6</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Turbs</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>All at start (comparison test case)</t>
+  </si>
+  <si>
+    <t>Half at start, half at end</t>
+  </si>
+  <si>
+    <t>End of every block</t>
+  </si>
+  <si>
+    <t>Every 3 months of work</t>
+  </si>
+  <si>
+    <t>Equal every month</t>
+  </si>
+  <si>
+    <t>Separate</t>
+  </si>
+  <si>
+    <t>No Rescources</t>
+  </si>
+  <si>
+    <t>Overlap</t>
+  </si>
+  <si>
+    <t>Duration x Turbines</t>
+  </si>
+  <si>
+    <t>Windfarm Size</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>(later?)</t>
   </si>
 </sst>
 </file>
@@ -134,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +264,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,16 +298,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -482,7 +646,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,350 +994,502 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AD7D99-8775-4118-A1C8-7FD1490F7E75}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <f>COUNTIF(C11:G17, "=y")</f>
+        <v>28</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <f>COUNTIF(D11:G17, "=y")</f>
+        <v>25</v>
+      </c>
+      <c r="N3">
+        <f>M3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="J8">
+        <f>PRODUCT(J2:J7)</f>
+        <v>2016</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="K8:N8" si="0">PRODUCT(L2:L7)</f>
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="P8">
+        <f>L8+M8+N8</f>
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>6</v>
       </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J6">
-        <f>PRODUCT(J2:J5)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>25</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ref="B14:F17" si="0">B$13/100*$H14</f>
-        <v>3.6</v>
-      </c>
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="H14">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>6.72</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>33.6</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="0"/>
-        <v>67.2</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>336</v>
-      </c>
-      <c r="H15">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="H16">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="H17">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <v>40</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
         <v>5</v>
       </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>2</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-      <c r="E22">
-        <v>8</v>
-      </c>
-      <c r="F22">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
         <v>10</v>
       </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-      <c r="H22">
-        <v>10</v>
-      </c>
-      <c r="I22">
-        <v>10</v>
-      </c>
-      <c r="J22">
-        <v>10</v>
-      </c>
-      <c r="K22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23">
-        <v>20</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C11:G17 G18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated testcase generation (still bugs)
</commit_message>
<xml_diff>
--- a/Code/Overlap/Input Files/Experiment setups.xlsx
+++ b/Code/Overlap/Input Files/Experiment setups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1812D8E-58E3-4977-B5E5-A22E9F6FAEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39944384-9704-4C1A-BAE9-FE9FBBF511AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attempt 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Variable</t>
   </si>
@@ -121,18 +121,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>Wave</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>(None)</t>
-  </si>
-  <si>
     <t>All (None)</t>
   </si>
   <si>
@@ -220,10 +208,7 @@
     <t>Windfarm Size</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>(later?)</t>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -994,10 +979,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AD7D99-8775-4118-A1C8-7FD1490F7E75}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A26" sqref="A26:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,18 +1005,18 @@
         <v>1</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1040,33 +1025,33 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
@@ -1124,19 +1109,19 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -1153,7 +1138,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>80</v>
@@ -1187,7 +1172,7 @@
         <v>2016</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="K8:N8" si="0">PRODUCT(L2:L7)</f>
+        <f t="shared" ref="L8:N8" si="0">PRODUCT(L2:L7)</f>
         <v>12</v>
       </c>
       <c r="M8">
@@ -1206,7 +1191,7 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1218,19 +1203,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
@@ -1241,22 +1226,22 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1264,68 +1249,68 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1333,68 +1318,68 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1410,31 +1395,31 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1442,43 +1427,12 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <v>15</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11:G17 G18">

</xml_diff>

<commit_message>
Fixed bugs in new test generation
</commit_message>
<xml_diff>
--- a/Code/Overlap/Input Files/Experiment setups.xlsx
+++ b/Code/Overlap/Input Files/Experiment setups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39944384-9704-4C1A-BAE9-FE9FBBF511AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986F23BA-5BD0-407D-9C98-3C8AB9A87F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
+    <workbookView minimized="1" xWindow="31260" yWindow="150" windowWidth="14400" windowHeight="11385" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attempt 1" sheetId="1" r:id="rId1"/>
@@ -982,7 +982,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C29"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Gantt, models, base test cases
</commit_message>
<xml_diff>
--- a/Code/Overlap/Input Files/Experiment setups.xlsx
+++ b/Code/Overlap/Input Files/Experiment setups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986F23BA-5BD0-407D-9C98-3C8AB9A87F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1143DC4F-B74B-4BFD-B01E-06BD5080C3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31260" yWindow="150" windowWidth="14400" windowHeight="11385" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2C11222A-7ED6-4012-9D9D-010458C3198B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attempt 1" sheetId="1" r:id="rId1"/>
@@ -982,7 +982,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,6 +1243,9 @@
       <c r="G11" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1266,6 +1269,9 @@
       <c r="G12" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1289,6 +1295,9 @@
       <c r="G13" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H13" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1312,6 +1321,9 @@
       <c r="G14" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H14">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1335,6 +1347,9 @@
       <c r="G15" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1358,8 +1373,11 @@
       <c r="G16" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1381,16 +1399,19 @@
       <c r="G17" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1419,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1406,7 +1427,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1414,7 +1435,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1422,7 +1443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1430,7 +1451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>

</xml_diff>